<commit_message>
update postcard  HK-846298 content
</commit_message>
<xml_diff>
--- a/template/postcardStory.xlsx
+++ b/template/postcardStory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\web\Postcrossing_map_generator\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9505D903-0936-4708-BBA8-2433DCE34EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF61677-9B46-4D6F-A783-73B50DB6C652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="540" windowWidth="17280" windowHeight="10716" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t>content_cn</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -783,6 +783,18 @@
   </si>
   <si>
     <t>“非常感谢您提供的https://www.bgi.com 的参考资料。我非常有兴趣阅读这个网站，了解基因组学和生物信息学作为我所主修科学的分支。祝您一切顺利！”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HK-846298</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你的女儿很可爱！我找到这张粉红色的猫猫postcard，闪闪的，希望她会喜欢！祝圣诞快乐！新年进步！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你的女兒很可愛！ 我找到這張粉紅色的貓貓postcard，閃閃的，希望她會喜歡！ 祝聖誕快樂！ 新年進步！</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -860,11 +872,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1148,29 +1157,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D26" sqref="D26:E26"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="18.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.08203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.4140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.75" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.9140625" style="1"/>
+    <col min="1" max="1" width="19.109375" style="1" customWidth="1"/>
+    <col min="2" max="3" width="52.44140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1180,278 +1188,278 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="94.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="94.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -1461,92 +1469,103 @@
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="58.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="58.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="153.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="18.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="1" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>